<commit_message>
Updated the driver trend analysis again.
</commit_message>
<xml_diff>
--- a/Outputs/LT_equationsToPercentChangePerYr_drivers_updated.xlsx
+++ b/Outputs/LT_equationsToPercentChangePerYr_drivers_updated.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/40436072c29b51f3/University of Johannesburg/Post-Doc/Nature Research Centre/How Changes in Bioversity Change Biodiversity/Analyses/Biochange_Paper1/Outputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{94DB7288-2E27-431B-80FE-6BA4C2518901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="107" documentId="13_ncr:40009_{94DB7288-2E27-431B-80FE-6BA4C2518901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8ED4F924-F2E6-48D0-BFF1-05FB1457F1E0}"/>
   <bookViews>
-    <workbookView xWindow="45972" yWindow="7920" windowWidth="23256" windowHeight="12456"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LT_Yr_metaanaly_weighted_noRand" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>Response</t>
   </si>
@@ -52,18 +65,9 @@
     <t>tranformation</t>
   </si>
   <si>
-    <t>OverallChange</t>
-  </si>
-  <si>
     <t>PercentChange</t>
   </si>
   <si>
-    <t>log10</t>
-  </si>
-  <si>
-    <t>log10 + 3.5</t>
-  </si>
-  <si>
     <t>none</t>
   </si>
   <si>
@@ -74,15 +78,36 @@
   </si>
   <si>
     <t>mg/L</t>
+  </si>
+  <si>
+    <t>log10 + 0.1</t>
+  </si>
+  <si>
+    <t>SI Unit</t>
+  </si>
+  <si>
+    <t>CorrectedEst</t>
+  </si>
+  <si>
+    <t>Number of years</t>
+  </si>
+  <si>
+    <t>Overall change</t>
+  </si>
+  <si>
+    <t>log10 + 0.02</t>
+  </si>
+  <si>
+    <t>SI Unit Change per YR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="173" formatCode="0.000"/>
-    <numFmt numFmtId="191" formatCode="0.0000000000000000000000000"/>
+    <numFmt numFmtId="164" formatCode="0.0000000000000000000000000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -226,7 +251,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -404,6 +429,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -567,13 +598,16 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="191" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -928,24 +962,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="8.15625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.26171875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.05078125" customWidth="1"/>
-    <col min="4" max="4" width="12.9453125" customWidth="1"/>
-    <col min="5" max="5" width="12.578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.15625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.26171875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.62890625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.62890625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.89453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.89453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5234375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.62890625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.89453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.3671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -959,158 +996,219 @@
         <v>9</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F1" t="s">
         <v>10</v>
       </c>
+      <c r="G1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2">
-        <v>-5.9159304034355504E-3</v>
+        <v>-1.9313704314662501E-3</v>
       </c>
       <c r="C2">
         <v>85.494129999999998</v>
       </c>
       <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="4">
+        <f>(10^B2-1)</f>
+        <v>-4.4372708585844745E-3</v>
+      </c>
+      <c r="F2" s="1">
+        <f>E2*100</f>
+        <v>-0.44372708585844745</v>
+      </c>
+      <c r="G2" s="1">
+        <f>C2*(F2/100)</f>
+        <v>-0.37936061162903267</v>
+      </c>
+      <c r="H2">
+        <v>11</v>
+      </c>
+      <c r="I2" s="1">
+        <f>G2*H2</f>
+        <v>-4.1729667279193592</v>
+      </c>
+      <c r="J2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="2">
-        <f>(10^B2-1)*100</f>
-        <v>-1.3529574470233618</v>
-      </c>
-      <c r="F2" s="2">
-        <f>(10^B2-1)*C2</f>
-        <v>-1.1566991986028341</v>
-      </c>
-      <c r="G2" t="s">
-        <v>15</v>
-      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3">
-        <v>5.5966571209545402E-2</v>
+        <v>4.3954203125064997E-2</v>
       </c>
       <c r="C3">
         <v>9.7851169999999996</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="2">
-        <f>(B3/C3)*100</f>
-        <v>0.57195607583992503</v>
-      </c>
-      <c r="F3" s="2">
-        <f>B3*C3</f>
-        <v>0.5476394473742332</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
+      </c>
+      <c r="E3" s="4">
+        <f>B3/C3</f>
+        <v>4.4919445649004505E-3</v>
+      </c>
+      <c r="F3" s="1">
+        <f>E3*100</f>
+        <v>0.44919445649004508</v>
+      </c>
+      <c r="G3" s="1">
+        <f t="shared" ref="G3:G6" si="0">C3*(F3/100)</f>
+        <v>4.3954203125064997E-2</v>
+      </c>
+      <c r="H3">
+        <v>11</v>
+      </c>
+      <c r="I3" s="1">
+        <f t="shared" ref="I3:I6" si="1">G3*H3</f>
+        <v>0.48349623437571498</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4">
-        <v>1.42428601990017E-2</v>
+        <v>1.4976122087730999E-2</v>
       </c>
       <c r="C4">
         <v>8.1378430000000002</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="2">
-        <f>(B4/C4)*100</f>
-        <v>0.17502009069235791</v>
-      </c>
-      <c r="F4" s="2">
-        <f>B4*C4</f>
-        <v>0.1159061601704246</v>
+        <v>11</v>
+      </c>
+      <c r="E4" s="4">
+        <f t="shared" ref="E4:E5" si="2">B4/C4</f>
+        <v>1.8403060968036615E-3</v>
+      </c>
+      <c r="F4" s="1">
+        <f t="shared" ref="F4:F5" si="3">E4*100</f>
+        <v>0.18403060968036616</v>
+      </c>
+      <c r="G4" s="1">
+        <f t="shared" si="0"/>
+        <v>1.4976122087730999E-2</v>
+      </c>
+      <c r="H4">
+        <v>11</v>
+      </c>
+      <c r="I4" s="1">
+        <f t="shared" si="1"/>
+        <v>0.164737342965041</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5">
-        <v>0.13274183726983499</v>
+        <v>0.118568076525986</v>
       </c>
       <c r="C5">
         <v>9.5775699999999997</v>
       </c>
       <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="4">
+        <f t="shared" si="2"/>
+        <v>1.2379766112488449E-2</v>
+      </c>
+      <c r="F5" s="1">
+        <f t="shared" si="3"/>
+        <v>1.2379766112488451</v>
+      </c>
+      <c r="G5" s="1">
+        <f t="shared" si="0"/>
+        <v>0.11856807652598601</v>
+      </c>
+      <c r="H5">
+        <v>11</v>
+      </c>
+      <c r="I5" s="1">
+        <f t="shared" si="1"/>
+        <v>1.3042488417858462</v>
+      </c>
+      <c r="J5" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="2">
-        <f>(B5/C5)*100</f>
-        <v>1.3859657227233524</v>
-      </c>
-      <c r="F5" s="2">
-        <f>B5*C5</f>
-        <v>1.2713442383804534</v>
-      </c>
-      <c r="G5" t="s">
-        <v>17</v>
-      </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6">
-        <v>-1.7223328382309701E-2</v>
+        <v>-1.2587680250102699E-2</v>
       </c>
       <c r="C6">
         <v>7.6691300000000004E-2</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="2">
-        <f>(10^B6-1)*100</f>
-        <v>-3.888208688197492</v>
+        <v>20</v>
+      </c>
+      <c r="E6" s="4">
+        <f>(10^B6-1)</f>
+        <v>-2.8568191791302766E-2</v>
       </c>
       <c r="F6" s="1">
-        <f>B6*C6</f>
-        <v>-1.320879443966228E-3</v>
-      </c>
-      <c r="G6" t="s">
-        <v>17</v>
+        <f>E6*100</f>
+        <v>-2.8568191791302766</v>
+      </c>
+      <c r="G6" s="1">
+        <f t="shared" si="0"/>
+        <v>-2.1909317671243381E-3</v>
+      </c>
+      <c r="H6">
+        <v>11</v>
+      </c>
+      <c r="I6" s="1">
+        <f t="shared" si="1"/>
+        <v>-2.4100249438367721E-2</v>
+      </c>
+      <c r="J6" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7">
-        <v>2.8467535040250301E-3</v>
-      </c>
-      <c r="C7" s="4">
-        <v>3.2431790000000001E-18</v>
-      </c>
-      <c r="D7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="2">
-        <f>(10^B7-3.5)*100</f>
-        <v>-249.34235774951716</v>
-      </c>
-      <c r="F7" s="2">
-        <f>(10^B7-3.5)*C7</f>
-        <v>-8.086618984637214E-18</v>
-      </c>
+        <v>6.4824076123632902E-3</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="5"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="F9" s="5"/>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="E9" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Reran driver analyses for nutrients and created a figure of the nutrients included in the PCA axis 1.
</commit_message>
<xml_diff>
--- a/Outputs/LT_equationsToPercentChangePerYr_drivers_updated.xlsx
+++ b/Outputs/LT_equationsToPercentChangePerYr_drivers_updated.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/40436072c29b51f3/University of Johannesburg/Post-Doc/Nature Research Centre/How Changes in Bioversity Change Biodiversity/Analyses/Biochange_Paper1/Outputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="107" documentId="13_ncr:40009_{94DB7288-2E27-431B-80FE-6BA4C2518901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8ED4F924-F2E6-48D0-BFF1-05FB1457F1E0}"/>
+  <xr:revisionPtr revIDLastSave="185" documentId="13_ncr:40009_{94DB7288-2E27-431B-80FE-6BA4C2518901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{626E2499-0DF0-427D-A4C9-553794360D57}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LT_Yr_metaanaly_weighted_noRand" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="32">
   <si>
     <t>Response</t>
   </si>
@@ -99,15 +99,64 @@
   </si>
   <si>
     <t>SI Unit Change per YR</t>
+  </si>
+  <si>
+    <t>alkalinity</t>
+  </si>
+  <si>
+    <t>EC</t>
+  </si>
+  <si>
+    <t>NO3.N</t>
+  </si>
+  <si>
+    <t>NO2.N</t>
+  </si>
+  <si>
+    <t>mineral.N</t>
+  </si>
+  <si>
+    <t>Tot.N</t>
+  </si>
+  <si>
+    <t>PO4.P</t>
+  </si>
+  <si>
+    <t>Tot.P</t>
+  </si>
+  <si>
+    <t>mmol/L</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>µ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>S/cm</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="0.0000000000000000000000000"/>
+  <numFmts count="3">
     <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="171" formatCode="0.0000"/>
+    <numFmt numFmtId="179" formatCode="0.000000000000"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -598,16 +647,15 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="11" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -963,26 +1011,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="A7" sqref="A7:J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.26171875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.62890625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.62890625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.89453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.89453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5234375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.62890625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.89453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.3671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1014,7 +1062,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1027,7 +1075,7 @@
       <c r="D2" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="3">
         <f>(10^B2-1)</f>
         <v>-4.4372708585844745E-3</v>
       </c>
@@ -1035,22 +1083,22 @@
         <f>E2*100</f>
         <v>-0.44372708585844745</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2" s="6">
         <f>C2*(F2/100)</f>
         <v>-0.37936061162903267</v>
       </c>
       <c r="H2">
         <v>11</v>
       </c>
-      <c r="I2" s="1">
-        <f>G2*H2</f>
+      <c r="I2" s="5">
+        <f t="shared" ref="I2:I6" si="0">G2*H2</f>
         <v>-4.1729667279193592</v>
       </c>
       <c r="J2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1063,30 +1111,30 @@
       <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <f>B3/C3</f>
         <v>4.4919445649004505E-3</v>
       </c>
       <c r="F3" s="1">
-        <f>E3*100</f>
+        <f t="shared" ref="F3:F15" si="1">E3*100</f>
         <v>0.44919445649004508</v>
       </c>
-      <c r="G3" s="1">
-        <f t="shared" ref="G3:G6" si="0">C3*(F3/100)</f>
+      <c r="G3" s="6">
+        <f t="shared" ref="G3:G6" si="2">C3*(F3/100)</f>
         <v>4.3954203125064997E-2</v>
       </c>
       <c r="H3">
         <v>11</v>
       </c>
-      <c r="I3" s="1">
-        <f t="shared" ref="I3:I6" si="1">G3*H3</f>
+      <c r="I3" s="5">
+        <f t="shared" si="0"/>
         <v>0.48349623437571498</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1099,27 +1147,27 @@
       <c r="D4" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="4">
-        <f t="shared" ref="E4:E5" si="2">B4/C4</f>
+      <c r="E4" s="3">
+        <f>B4/C4</f>
         <v>1.8403060968036615E-3</v>
       </c>
       <c r="F4" s="1">
-        <f t="shared" ref="F4:F5" si="3">E4*100</f>
+        <f t="shared" si="1"/>
         <v>0.18403060968036616</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" s="6">
+        <f t="shared" si="2"/>
+        <v>1.4976122087730999E-2</v>
+      </c>
+      <c r="H4">
+        <v>11</v>
+      </c>
+      <c r="I4" s="5">
         <f t="shared" si="0"/>
-        <v>1.4976122087730999E-2</v>
-      </c>
-      <c r="H4">
-        <v>11</v>
-      </c>
-      <c r="I4" s="1">
-        <f t="shared" si="1"/>
         <v>0.164737342965041</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1132,30 +1180,30 @@
       <c r="D5" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="3">
+        <f>B5/C5</f>
+        <v>1.2379766112488449E-2</v>
+      </c>
+      <c r="F5" s="1">
+        <f t="shared" si="1"/>
+        <v>1.2379766112488451</v>
+      </c>
+      <c r="G5" s="6">
         <f t="shared" si="2"/>
-        <v>1.2379766112488449E-2</v>
-      </c>
-      <c r="F5" s="1">
-        <f t="shared" si="3"/>
-        <v>1.2379766112488451</v>
-      </c>
-      <c r="G5" s="1">
+        <v>0.11856807652598601</v>
+      </c>
+      <c r="H5">
+        <v>11</v>
+      </c>
+      <c r="I5" s="5">
         <f t="shared" si="0"/>
-        <v>0.11856807652598601</v>
-      </c>
-      <c r="H5">
-        <v>11</v>
-      </c>
-      <c r="I5" s="1">
-        <f t="shared" si="1"/>
         <v>1.3042488417858462</v>
       </c>
       <c r="J5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1168,47 +1216,332 @@
       <c r="D6" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="3">
         <f>(10^B6-1)</f>
         <v>-2.8568191791302766E-2</v>
       </c>
       <c r="F6" s="1">
-        <f>E6*100</f>
+        <f t="shared" si="1"/>
         <v>-2.8568191791302766</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="6">
+        <f t="shared" si="2"/>
+        <v>-2.1909317671243381E-3</v>
+      </c>
+      <c r="H6">
+        <v>11</v>
+      </c>
+      <c r="I6" s="5">
         <f t="shared" si="0"/>
-        <v>-2.1909317671243381E-3</v>
-      </c>
-      <c r="H6">
-        <v>11</v>
-      </c>
-      <c r="I6" s="1">
-        <f t="shared" si="1"/>
         <v>-2.4100249438367721E-2</v>
       </c>
       <c r="J6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" t="s">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="4">
         <v>6.4824076123632902E-3</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="5"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="4"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="E9" s="3"/>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8">
+        <v>3.6452021478815801E-2</v>
+      </c>
+      <c r="C8">
+        <v>4.297974</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="3">
+        <f>B8/C8</f>
+        <v>8.481210328125717E-3</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="1"/>
+        <v>0.84812103281257167</v>
+      </c>
+      <c r="G8" s="6">
+        <f t="shared" ref="G8:G15" si="3">C8*(F8/100)</f>
+        <v>3.6452021478815801E-2</v>
+      </c>
+      <c r="H8">
+        <v>11</v>
+      </c>
+      <c r="I8" s="5">
+        <f t="shared" ref="I8:I15" si="4">G8*H8</f>
+        <v>0.40097223626697381</v>
+      </c>
+      <c r="J8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9">
+        <v>9.1306867732430098E-4</v>
+      </c>
+      <c r="C9">
+        <v>541.51559999999995</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="3">
+        <f>(10^B9-1)</f>
+        <v>2.1046299563469706E-3</v>
+      </c>
+      <c r="F9" s="1">
+        <f t="shared" si="1"/>
+        <v>0.21046299563469706</v>
+      </c>
+      <c r="G9" s="6">
+        <f t="shared" si="3"/>
+        <v>1.1396899535892036</v>
+      </c>
+      <c r="H9">
+        <v>11</v>
+      </c>
+      <c r="I9" s="5">
+        <f t="shared" si="4"/>
+        <v>12.536589489481239</v>
+      </c>
+      <c r="J9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10">
+        <v>1.8681400902442798E-2</v>
+      </c>
+      <c r="C10">
+        <v>1.8795040000000001</v>
+      </c>
+      <c r="D10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="3">
+        <f t="shared" ref="E10:E15" si="5">(10^B10-1)</f>
+        <v>4.3954091917202565E-2</v>
+      </c>
+      <c r="F10" s="1">
+        <f t="shared" si="1"/>
+        <v>4.3954091917202565</v>
+      </c>
+      <c r="G10" s="6">
+        <f t="shared" si="3"/>
+        <v>8.2611891574749893E-2</v>
+      </c>
+      <c r="H10">
+        <v>11</v>
+      </c>
+      <c r="I10" s="5">
+        <f t="shared" si="4"/>
+        <v>0.90873080732224887</v>
+      </c>
+      <c r="J10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11">
+        <v>-2.7079099530824102E-4</v>
+      </c>
+      <c r="C11">
+        <v>1.610435E-2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="3">
+        <f t="shared" si="5"/>
+        <v>-6.2332496134465121E-4</v>
+      </c>
+      <c r="F11" s="1">
+        <f t="shared" si="1"/>
+        <v>-6.2332496134465121E-2</v>
+      </c>
+      <c r="G11" s="6">
+        <f t="shared" si="3"/>
+        <v>-1.0038243341230734E-5</v>
+      </c>
+      <c r="H11">
+        <v>11</v>
+      </c>
+      <c r="I11" s="5">
+        <f t="shared" si="4"/>
+        <v>-1.1042067675353807E-4</v>
+      </c>
+      <c r="J11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12">
+        <v>1.5067410865642601E-2</v>
+      </c>
+      <c r="C12">
+        <v>1.9787429999999999</v>
+      </c>
+      <c r="D12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" si="5"/>
+        <v>3.5302853145080082E-2</v>
+      </c>
+      <c r="F12" s="1">
+        <f t="shared" si="1"/>
+        <v>3.5302853145080082</v>
+      </c>
+      <c r="G12" s="6">
+        <f t="shared" si="3"/>
+        <v>6.9855273540855189E-2</v>
+      </c>
+      <c r="H12">
+        <v>11</v>
+      </c>
+      <c r="I12" s="5">
+        <f t="shared" si="4"/>
+        <v>0.76840800894940708</v>
+      </c>
+      <c r="J12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13">
+        <v>8.3816036615180292E-3</v>
+      </c>
+      <c r="C13">
+        <v>2.7824430000000002</v>
+      </c>
+      <c r="D13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="3">
+        <f t="shared" si="5"/>
+        <v>1.9486792069553394E-2</v>
+      </c>
+      <c r="F13" s="1">
+        <f t="shared" si="1"/>
+        <v>1.9486792069553394</v>
+      </c>
+      <c r="G13" s="6">
+        <f t="shared" si="3"/>
+        <v>5.4220888186384354E-2</v>
+      </c>
+      <c r="H13">
+        <v>11</v>
+      </c>
+      <c r="I13" s="5">
+        <f t="shared" si="4"/>
+        <v>0.5964297700502279</v>
+      </c>
+      <c r="J13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14">
+        <v>-1.54712427761869E-3</v>
+      </c>
+      <c r="C14">
+        <v>6.1834779999999999E-2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" si="5"/>
+        <v>-3.5560475322348184E-3</v>
+      </c>
+      <c r="F14" s="1">
+        <f t="shared" si="1"/>
+        <v>-0.35560475322348184</v>
+      </c>
+      <c r="G14" s="6">
+        <f t="shared" si="3"/>
+        <v>-2.1988741682528291E-4</v>
+      </c>
+      <c r="H14">
+        <v>11</v>
+      </c>
+      <c r="I14" s="5">
+        <f t="shared" si="4"/>
+        <v>-2.418761585078112E-3</v>
+      </c>
+      <c r="J14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15">
+        <v>-2.3823991712979401E-3</v>
+      </c>
+      <c r="C15">
+        <v>0.10491739999999999</v>
+      </c>
+      <c r="D15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="3">
+        <f t="shared" si="5"/>
+        <v>-5.4706579677210598E-3</v>
+      </c>
+      <c r="F15" s="1">
+        <f t="shared" si="1"/>
+        <v>-0.54706579677210598</v>
+      </c>
+      <c r="G15" s="6">
+        <f t="shared" si="3"/>
+        <v>-5.7396721026257752E-4</v>
+      </c>
+      <c r="H15">
+        <v>11</v>
+      </c>
+      <c r="I15" s="5">
+        <f t="shared" si="4"/>
+        <v>-6.3136393128883526E-3</v>
+      </c>
+      <c r="J15" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated driver analyses. Tried factorised meta-analyses.
</commit_message>
<xml_diff>
--- a/Outputs/LT_equationsToPercentChangePerYr_drivers_updated.xlsx
+++ b/Outputs/LT_equationsToPercentChangePerYr_drivers_updated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/40436072c29b51f3/University of Johannesburg/Post-Doc/Nature Research Centre/How Changes in Bioversity Change Biodiversity/Analyses/Biochange_Paper1/Outputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="185" documentId="13_ncr:40009_{94DB7288-2E27-431B-80FE-6BA4C2518901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{626E2499-0DF0-427D-A4C9-553794360D57}"/>
+  <xr:revisionPtr revIDLastSave="207" documentId="13_ncr:40009_{94DB7288-2E27-431B-80FE-6BA4C2518901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CDE8AFFB-BF66-48E5-8D5C-0DF15A4394B0}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LT_Yr_metaanaly_weighted_noRand" sheetId="1" r:id="rId1"/>
@@ -154,9 +154,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="171" formatCode="0.0000"/>
-    <numFmt numFmtId="179" formatCode="0.000000000000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000000000000"/>
+    <numFmt numFmtId="167" formatCode="0.0000"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -651,11 +651,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1014,7 +1014,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:J7"/>
+      <selection activeCell="I15" sqref="I2:I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1083,14 +1083,14 @@
         <f>E2*100</f>
         <v>-0.44372708585844745</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="5">
         <f>C2*(F2/100)</f>
         <v>-0.37936061162903267</v>
       </c>
       <c r="H2">
         <v>11</v>
       </c>
-      <c r="I2" s="5">
+      <c r="I2" s="6">
         <f t="shared" ref="I2:I6" si="0">G2*H2</f>
         <v>-4.1729667279193592</v>
       </c>
@@ -1119,14 +1119,14 @@
         <f t="shared" ref="F3:F15" si="1">E3*100</f>
         <v>0.44919445649004508</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="5">
         <f t="shared" ref="G3:G6" si="2">C3*(F3/100)</f>
         <v>4.3954203125064997E-2</v>
       </c>
       <c r="H3">
         <v>11</v>
       </c>
-      <c r="I3" s="5">
+      <c r="I3" s="6">
         <f t="shared" si="0"/>
         <v>0.48349623437571498</v>
       </c>
@@ -1155,14 +1155,14 @@
         <f t="shared" si="1"/>
         <v>0.18403060968036616</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="5">
         <f t="shared" si="2"/>
         <v>1.4976122087730999E-2</v>
       </c>
       <c r="H4">
         <v>11</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="6">
         <f t="shared" si="0"/>
         <v>0.164737342965041</v>
       </c>
@@ -1188,14 +1188,14 @@
         <f t="shared" si="1"/>
         <v>1.2379766112488451</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="5">
         <f t="shared" si="2"/>
         <v>0.11856807652598601</v>
       </c>
       <c r="H5">
         <v>11</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="6">
         <f t="shared" si="0"/>
         <v>1.3042488417858462</v>
       </c>
@@ -1224,14 +1224,14 @@
         <f t="shared" si="1"/>
         <v>-2.8568191791302766</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="5">
         <f t="shared" si="2"/>
         <v>-2.1909317671243381E-3</v>
       </c>
       <c r="H6">
         <v>11</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="6">
         <f t="shared" si="0"/>
         <v>-2.4100249438367721E-2</v>
       </c>
@@ -1276,14 +1276,14 @@
         <f t="shared" si="1"/>
         <v>0.84812103281257167</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="5">
         <f t="shared" ref="G8:G15" si="3">C8*(F8/100)</f>
         <v>3.6452021478815801E-2</v>
       </c>
       <c r="H8">
         <v>11</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I8" s="6">
         <f t="shared" ref="I8:I15" si="4">G8*H8</f>
         <v>0.40097223626697381</v>
       </c>
@@ -1312,14 +1312,14 @@
         <f t="shared" si="1"/>
         <v>0.21046299563469706</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="5">
         <f t="shared" si="3"/>
         <v>1.1396899535892036</v>
       </c>
       <c r="H9">
         <v>11</v>
       </c>
-      <c r="I9" s="5">
+      <c r="I9" s="6">
         <f t="shared" si="4"/>
         <v>12.536589489481239</v>
       </c>
@@ -1348,14 +1348,14 @@
         <f t="shared" si="1"/>
         <v>4.3954091917202565</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G10" s="5">
         <f t="shared" si="3"/>
         <v>8.2611891574749893E-2</v>
       </c>
       <c r="H10">
         <v>11</v>
       </c>
-      <c r="I10" s="5">
+      <c r="I10" s="6">
         <f t="shared" si="4"/>
         <v>0.90873080732224887</v>
       </c>
@@ -1384,14 +1384,14 @@
         <f t="shared" si="1"/>
         <v>-6.2332496134465121E-2</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G11" s="5">
         <f t="shared" si="3"/>
         <v>-1.0038243341230734E-5</v>
       </c>
       <c r="H11">
         <v>11</v>
       </c>
-      <c r="I11" s="5">
+      <c r="I11" s="6">
         <f t="shared" si="4"/>
         <v>-1.1042067675353807E-4</v>
       </c>
@@ -1420,14 +1420,14 @@
         <f t="shared" si="1"/>
         <v>3.5302853145080082</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G12" s="5">
         <f t="shared" si="3"/>
         <v>6.9855273540855189E-2</v>
       </c>
       <c r="H12">
         <v>11</v>
       </c>
-      <c r="I12" s="5">
+      <c r="I12" s="6">
         <f t="shared" si="4"/>
         <v>0.76840800894940708</v>
       </c>
@@ -1456,14 +1456,14 @@
         <f t="shared" si="1"/>
         <v>1.9486792069553394</v>
       </c>
-      <c r="G13" s="6">
+      <c r="G13" s="5">
         <f t="shared" si="3"/>
         <v>5.4220888186384354E-2</v>
       </c>
       <c r="H13">
         <v>11</v>
       </c>
-      <c r="I13" s="5">
+      <c r="I13" s="6">
         <f t="shared" si="4"/>
         <v>0.5964297700502279</v>
       </c>
@@ -1492,14 +1492,14 @@
         <f t="shared" si="1"/>
         <v>-0.35560475322348184</v>
       </c>
-      <c r="G14" s="6">
+      <c r="G14" s="5">
         <f t="shared" si="3"/>
         <v>-2.1988741682528291E-4</v>
       </c>
       <c r="H14">
         <v>11</v>
       </c>
-      <c r="I14" s="5">
+      <c r="I14" s="6">
         <f t="shared" si="4"/>
         <v>-2.418761585078112E-3</v>
       </c>
@@ -1528,14 +1528,14 @@
         <f t="shared" si="1"/>
         <v>-0.54706579677210598</v>
       </c>
-      <c r="G15" s="6">
+      <c r="G15" s="5">
         <f t="shared" si="3"/>
         <v>-5.7396721026257752E-4</v>
       </c>
       <c r="H15">
         <v>11</v>
       </c>
-      <c r="I15" s="5">
+      <c r="I15" s="6">
         <f t="shared" si="4"/>
         <v>-6.3136393128883526E-3</v>
       </c>

</xml_diff>

<commit_message>
slightly modified code. determined how species changed through time with regards to abundance and site distribution.
</commit_message>
<xml_diff>
--- a/Outputs/LT_equationsToPercentChangePerYr_drivers_updated.xlsx
+++ b/Outputs/LT_equationsToPercentChangePerYr_drivers_updated.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/40436072c29b51f3/University of Johannesburg/Post-Doc/Nature Research Centre/How Changes in Bioversity Change Biodiversity/Analyses/Biochange_Paper1/Outputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="207" documentId="13_ncr:40009_{94DB7288-2E27-431B-80FE-6BA4C2518901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CDE8AFFB-BF66-48E5-8D5C-0DF15A4394B0}"/>
+  <xr:revisionPtr revIDLastSave="209" documentId="13_ncr:40009_{94DB7288-2E27-431B-80FE-6BA4C2518901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC8E94CE-1BE3-4961-A85F-5CB452E98CE7}"/>
   <bookViews>
     <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -153,10 +153,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.000000000000"/>
-    <numFmt numFmtId="167" formatCode="0.0000"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -647,15 +646,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -715,9 +713,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -755,7 +753,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -861,7 +859,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1003,7 +1001,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1014,7 +1012,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I2:I15"/>
+      <selection activeCell="I2" sqref="I2:I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1090,7 +1088,7 @@
       <c r="H2">
         <v>11</v>
       </c>
-      <c r="I2" s="6">
+      <c r="I2" s="1">
         <f t="shared" ref="I2:I6" si="0">G2*H2</f>
         <v>-4.1729667279193592</v>
       </c>
@@ -1126,7 +1124,7 @@
       <c r="H3">
         <v>11</v>
       </c>
-      <c r="I3" s="6">
+      <c r="I3" s="1">
         <f t="shared" si="0"/>
         <v>0.48349623437571498</v>
       </c>
@@ -1162,7 +1160,7 @@
       <c r="H4">
         <v>11</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="1">
         <f t="shared" si="0"/>
         <v>0.164737342965041</v>
       </c>
@@ -1195,7 +1193,7 @@
       <c r="H5">
         <v>11</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I5" s="1">
         <f t="shared" si="0"/>
         <v>1.3042488417858462</v>
       </c>
@@ -1231,7 +1229,7 @@
       <c r="H6">
         <v>11</v>
       </c>
-      <c r="I6" s="6">
+      <c r="I6" s="1">
         <f t="shared" si="0"/>
         <v>-2.4100249438367721E-2</v>
       </c>
@@ -1252,7 +1250,7 @@
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
-      <c r="I7" s="7"/>
+      <c r="I7" s="6"/>
       <c r="J7" s="4"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
@@ -1283,7 +1281,7 @@
       <c r="H8">
         <v>11</v>
       </c>
-      <c r="I8" s="6">
+      <c r="I8" s="1">
         <f t="shared" ref="I8:I15" si="4">G8*H8</f>
         <v>0.40097223626697381</v>
       </c>
@@ -1319,7 +1317,7 @@
       <c r="H9">
         <v>11</v>
       </c>
-      <c r="I9" s="6">
+      <c r="I9" s="1">
         <f t="shared" si="4"/>
         <v>12.536589489481239</v>
       </c>
@@ -1355,7 +1353,7 @@
       <c r="H10">
         <v>11</v>
       </c>
-      <c r="I10" s="6">
+      <c r="I10" s="1">
         <f t="shared" si="4"/>
         <v>0.90873080732224887</v>
       </c>
@@ -1391,7 +1389,7 @@
       <c r="H11">
         <v>11</v>
       </c>
-      <c r="I11" s="6">
+      <c r="I11" s="1">
         <f t="shared" si="4"/>
         <v>-1.1042067675353807E-4</v>
       </c>
@@ -1427,7 +1425,7 @@
       <c r="H12">
         <v>11</v>
       </c>
-      <c r="I12" s="6">
+      <c r="I12" s="1">
         <f t="shared" si="4"/>
         <v>0.76840800894940708</v>
       </c>
@@ -1463,7 +1461,7 @@
       <c r="H13">
         <v>11</v>
       </c>
-      <c r="I13" s="6">
+      <c r="I13" s="1">
         <f t="shared" si="4"/>
         <v>0.5964297700502279</v>
       </c>
@@ -1499,7 +1497,7 @@
       <c r="H14">
         <v>11</v>
       </c>
-      <c r="I14" s="6">
+      <c r="I14" s="1">
         <f t="shared" si="4"/>
         <v>-2.418761585078112E-3</v>
       </c>
@@ -1535,7 +1533,7 @@
       <c r="H15">
         <v>11</v>
       </c>
-      <c r="I15" s="6">
+      <c r="I15" s="1">
         <f t="shared" si="4"/>
         <v>-6.3136393128883526E-3</v>
       </c>

</xml_diff>

<commit_message>
updated the plots looking at changes in individual species abundances through time. deleted old plots that were too chaotic.
</commit_message>
<xml_diff>
--- a/Outputs/LT_equationsToPercentChangePerYr_drivers_updated.xlsx
+++ b/Outputs/LT_equationsToPercentChangePerYr_drivers_updated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/40436072c29b51f3/University of Johannesburg/Post-Doc/Nature Research Centre/How Changes in Bioversity Change Biodiversity/Analyses/Biochange_Paper1/Outputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="209" documentId="13_ncr:40009_{94DB7288-2E27-431B-80FE-6BA4C2518901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC8E94CE-1BE3-4961-A85F-5CB452E98CE7}"/>
+  <xr:revisionPtr revIDLastSave="215" documentId="13_ncr:40009_{94DB7288-2E27-431B-80FE-6BA4C2518901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{83E864D3-0A30-4477-93DF-ED86545E9D3E}"/>
   <bookViews>
     <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="32">
   <si>
     <t>Response</t>
   </si>
@@ -1009,17 +1009,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I15"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="8.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.453125" customWidth="1"/>
     <col min="4" max="4" width="11.90625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.90625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.54296875" bestFit="1" customWidth="1"/>
@@ -1541,6 +1541,116 @@
         <v>14</v>
       </c>
     </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="1">
+        <v>85.494129999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="1">
+        <v>9.7851169999999996</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="1">
+        <v>8.1378430000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="1">
+        <v>9.5775699999999997</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="1">
+        <v>7.6691300000000004E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B22" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="1"/>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="1">
+        <v>4.297974</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="1">
+        <v>541.51559999999995</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" s="1">
+        <v>1.8795040000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B26" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" s="1">
+        <v>1.610435E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B27" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" s="1">
+        <v>1.9787429999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B28" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" s="1">
+        <v>2.7824430000000002</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B29" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29" s="1">
+        <v>6.1834779999999999E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B30" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30" s="1">
+        <v>0.10491739999999999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
recreated figures with smaller DPIs
</commit_message>
<xml_diff>
--- a/Outputs/LT_equationsToPercentChangePerYr_drivers_updated.xlsx
+++ b/Outputs/LT_equationsToPercentChangePerYr_drivers_updated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/40436072c29b51f3/University of Johannesburg/Post-Doc/Nature Research Centre/How Changes in Bioversity Change Biodiversity/Analyses/Biochange_Paper1/Outputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="218" documentId="13_ncr:40009_{94DB7288-2E27-431B-80FE-6BA4C2518901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{33C7B715-7A6E-41ED-B115-701D98BFEDEC}"/>
+  <xr:revisionPtr revIDLastSave="241" documentId="13_ncr:40009_{94DB7288-2E27-431B-80FE-6BA4C2518901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E27336B7-168C-4651-95CC-8F69F2EC5745}"/>
   <bookViews>
-    <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LT_Yr_metaanaly_weighted_noRand" sheetId="1" r:id="rId1"/>
@@ -153,9 +153,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="165" formatCode="0.000000000000"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -640,14 +639,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1006,20 +1002,20 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.453125" customWidth="1"/>
     <col min="4" max="4" width="11.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.6328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.90625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
@@ -1058,16 +1054,16 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>-1.9313704314662501E-3</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>85.494129999999998</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="1">
         <f>(10^B2-1)</f>
         <v>-4.4372708585844745E-3</v>
       </c>
@@ -1075,18 +1071,18 @@
         <f>E2*100</f>
         <v>-0.44372708585844745</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="1">
         <f>C2*(F2/100)</f>
         <v>-0.37936061162903267</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="3">
         <v>11</v>
       </c>
       <c r="I2" s="1">
         <f t="shared" ref="I2:I6" si="0">G2*H2</f>
         <v>-4.1729667279193592</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1094,32 +1090,32 @@
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>4.3954203125064997E-2</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>9.7851169999999996</v>
       </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="3">
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="1">
         <f>B3/C3</f>
         <v>4.4919445649004505E-3</v>
       </c>
       <c r="F3" s="1">
-        <f t="shared" ref="F3:F15" si="1">E3*100</f>
+        <f>E3*100</f>
         <v>0.44919445649004508</v>
       </c>
-      <c r="G3" s="4">
-        <f t="shared" ref="G3:G6" si="2">C3*(F3/100)</f>
+      <c r="G3" s="1">
+        <f>C3*(F3/100)</f>
         <v>4.3954203125064997E-2</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="3">
         <v>11</v>
       </c>
       <c r="I3" s="1">
-        <f t="shared" si="0"/>
+        <f>G3*H3</f>
         <v>0.48349623437571498</v>
       </c>
       <c r="J3" s="2" t="s">
@@ -1130,49 +1126,50 @@
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>1.4976122087730999E-2</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>8.1378430000000002</v>
       </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="3">
+      <c r="D4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="1">
         <f>B4/C4</f>
         <v>1.8403060968036615E-3</v>
       </c>
       <c r="F4" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="F4:F15" si="1">E4*100</f>
         <v>0.18403060968036616</v>
       </c>
-      <c r="G4" s="4">
-        <f t="shared" si="2"/>
+      <c r="G4" s="1">
+        <f t="shared" ref="G4:G6" si="2">C4*(F4/100)</f>
         <v>1.4976122087730999E-2</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="3">
         <v>11</v>
       </c>
       <c r="I4" s="1">
         <f t="shared" si="0"/>
         <v>0.164737342965041</v>
       </c>
+      <c r="J4" s="1"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>0.118568076525986</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>9.5775699999999997</v>
       </c>
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="3">
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="1">
         <f>B5/C5</f>
         <v>1.2379766112488449E-2</v>
       </c>
@@ -1180,18 +1177,18 @@
         <f t="shared" si="1"/>
         <v>1.2379766112488451</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="1">
         <f t="shared" si="2"/>
         <v>0.11856807652598601</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="3">
         <v>11</v>
       </c>
       <c r="I5" s="1">
         <f t="shared" si="0"/>
         <v>1.3042488417858462</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1199,16 +1196,16 @@
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>-1.2587680250102699E-2</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>7.6691300000000004E-2</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="1">
         <f>(10^B6-1)</f>
         <v>-2.8568191791302766E-2</v>
       </c>
@@ -1216,44 +1213,51 @@
         <f t="shared" si="1"/>
         <v>-2.8568191791302766</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="1">
         <f t="shared" si="2"/>
         <v>-2.1909317671243381E-3</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="3">
         <v>11</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" si="0"/>
         <v>-2.4100249438367721E-2</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="1">
         <v>6.4824076123632902E-3</v>
       </c>
-      <c r="I7" s="6"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>22</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>3.6452021478815801E-2</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
         <v>4.297974</v>
       </c>
-      <c r="D8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="3">
+      <c r="D8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="1">
         <f>B8/C8</f>
         <v>8.481210328125717E-3</v>
       </c>
@@ -1261,18 +1265,18 @@
         <f t="shared" si="1"/>
         <v>0.84812103281257167</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="1">
         <f t="shared" ref="G8:G15" si="3">C8*(F8/100)</f>
         <v>3.6452021478815801E-2</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="3">
         <v>11</v>
       </c>
       <c r="I8" s="1">
         <f t="shared" ref="I8:I15" si="4">G8*H8</f>
         <v>0.40097223626697381</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" s="1" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1280,16 +1284,16 @@
       <c r="A9" t="s">
         <v>23</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <v>9.1306867732430098E-4</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="1">
         <v>541.51559999999995</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="1">
         <f>(10^B9-1)</f>
         <v>2.1046299563469706E-3</v>
       </c>
@@ -1297,18 +1301,18 @@
         <f t="shared" si="1"/>
         <v>0.21046299563469706</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="1">
         <f t="shared" si="3"/>
         <v>1.1396899535892036</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="3">
         <v>11</v>
       </c>
       <c r="I9" s="1">
         <f t="shared" si="4"/>
         <v>12.536589489481239</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" s="1" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1316,16 +1320,16 @@
       <c r="A10" t="s">
         <v>24</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
         <v>1.8681400902442798E-2</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="1">
         <v>1.8795040000000001</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="1">
         <f t="shared" ref="E10:E15" si="5">(10^B10-1)</f>
         <v>4.3954091917202565E-2</v>
       </c>
@@ -1333,18 +1337,18 @@
         <f t="shared" si="1"/>
         <v>4.3954091917202565</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="1">
         <f t="shared" si="3"/>
         <v>8.2611891574749893E-2</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="3">
         <v>11</v>
       </c>
       <c r="I10" s="1">
         <f t="shared" si="4"/>
         <v>0.90873080732224887</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" s="1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1352,16 +1356,16 @@
       <c r="A11" t="s">
         <v>25</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <v>-2.7079099530824102E-4</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="1">
         <v>1.610435E-2</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="1">
         <f t="shared" si="5"/>
         <v>-6.2332496134465121E-4</v>
       </c>
@@ -1369,18 +1373,18 @@
         <f t="shared" si="1"/>
         <v>-6.2332496134465121E-2</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="1">
         <f t="shared" si="3"/>
         <v>-1.0038243341230734E-5</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="3">
         <v>11</v>
       </c>
       <c r="I11" s="1">
         <f t="shared" si="4"/>
         <v>-1.1042067675353807E-4</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J11" s="1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1388,16 +1392,16 @@
       <c r="A12" t="s">
         <v>26</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1">
         <v>1.5067410865642601E-2</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="1">
         <v>1.9787429999999999</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="1">
         <f t="shared" si="5"/>
         <v>3.5302853145080082E-2</v>
       </c>
@@ -1405,18 +1409,18 @@
         <f t="shared" si="1"/>
         <v>3.5302853145080082</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="1">
         <f t="shared" si="3"/>
         <v>6.9855273540855189E-2</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="3">
         <v>11</v>
       </c>
       <c r="I12" s="1">
         <f t="shared" si="4"/>
         <v>0.76840800894940708</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J12" s="1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1424,16 +1428,16 @@
       <c r="A13" t="s">
         <v>27</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="1">
         <v>8.3816036615180292E-3</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="1">
         <v>2.7824430000000002</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="1">
         <f t="shared" si="5"/>
         <v>1.9486792069553394E-2</v>
       </c>
@@ -1441,18 +1445,18 @@
         <f t="shared" si="1"/>
         <v>1.9486792069553394</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13" s="1">
         <f t="shared" si="3"/>
         <v>5.4220888186384354E-2</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="3">
         <v>11</v>
       </c>
       <c r="I13" s="1">
         <f t="shared" si="4"/>
         <v>0.5964297700502279</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J13" s="1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1460,16 +1464,16 @@
       <c r="A14" t="s">
         <v>28</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="1">
         <v>-1.54712427761869E-3</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="1">
         <v>6.1834779999999999E-2</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="1">
         <f t="shared" si="5"/>
         <v>-3.5560475322348184E-3</v>
       </c>
@@ -1477,18 +1481,18 @@
         <f t="shared" si="1"/>
         <v>-0.35560475322348184</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G14" s="1">
         <f t="shared" si="3"/>
         <v>-2.1988741682528291E-4</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="3">
         <v>11</v>
       </c>
       <c r="I14" s="1">
         <f t="shared" si="4"/>
         <v>-2.418761585078112E-3</v>
       </c>
-      <c r="J14" t="s">
+      <c r="J14" s="1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1496,16 +1500,16 @@
       <c r="A15" t="s">
         <v>29</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="1">
         <v>-2.3823991712979401E-3</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="1">
         <v>0.10491739999999999</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="1">
         <f t="shared" si="5"/>
         <v>-5.4706579677210598E-3</v>
       </c>
@@ -1513,18 +1517,18 @@
         <f t="shared" si="1"/>
         <v>-0.54706579677210598</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G15" s="1">
         <f t="shared" si="3"/>
         <v>-5.7396721026257752E-4</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="3">
         <v>11</v>
       </c>
       <c r="I15" s="1">
         <f t="shared" si="4"/>
         <v>-6.3136393128883526E-3</v>
       </c>
-      <c r="J15" t="s">
+      <c r="J15" s="1" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>